<commit_message>
Fix issue with Rules having double quotes
</commit_message>
<xml_diff>
--- a/DesignDocs/Rules.xlsx
+++ b/DesignDocs/Rules.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\BarbarianPrince\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\BarbarianPrince\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{99A9786C-5DAB-4C9D-A4A9-F6CBAE792ACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{037545BB-5C02-43E1-ADF0-C4B7BC71A83E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>

</xml_diff>

<commit_message>
Adding logging for SetButtonState() returning error.
</commit_message>
<xml_diff>
--- a/DesignDocs/Rules.xlsx
+++ b/DesignDocs/Rules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\BarbarianPrince\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{037545BB-5C02-43E1-ADF0-C4B7BC71A83E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E1F7898-0D2F-43D6-B2B9-DFA524662143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="1" r:id="rId1"/>
@@ -1025,20 +1025,6 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;&lt;Italic&gt;Poison Wounds:&lt;/Italic&gt; A poison wound cannot be healed in the normal manner. It remains a wound regardless of rest taken, until either a special possession provides a cure, or the charcter dies of wounds.</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r205 Lost&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Each time you attempt to leave a hex, there is a danger of becoming lost. Consult the Travel Table
- &lt;InlineUIContainer&gt;&lt;Button Name='myButtonT207' Content='t207' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
- and find the terrain type you are leaving. Read across to the 'Lost" column entry. Roll two die. If the dice total equals or exceeds the chart's number, your party is lost. If you move more than one hex in a day, you must check for getting lost before each move, i.e., before you enter the new hex.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;If you get lost, you cannot move further that day. You are stuck in the hex you tried to leave. You must check for a travel event unless performing self-guiding moves
- &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR205b' Content='r205b' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
- The travel check is performed in the hex you tried to enter, as if you actually entered it. This reflects you wondering around the edges of the new hex and perhaps encountering something.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR205a' Content='r205a' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Local Guide&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR205b1' Content='r205b' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Self-Guiding Moves&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR205c' Content='r205c' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Airborne&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR205d' Content='r205d' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; River Crossing</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;r343 Victim Selection&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;One character in your party is the victim or target of an attack. If your party is just you, then you are the target.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;Otherwise, select characters in your party one by one in any order you choose. When you select a character, roll one die. If the result is six, the character is the target.
@@ -3282,6 +3268,20 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;If you bring this possession to any hex north of the, you will command instant obedience throughout the Norhlands, regain your throne, and win the game! 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
               &lt;InlineUIContainer&gt;&lt;Image Source='../images/Staff.gif' Height='300' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r205 Lost&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Each time you attempt to leave a hex, there is a danger of becoming lost. Consult the Travel Table
+ &lt;InlineUIContainer&gt;&lt;Button Name='myButtonT207' Content='t207' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+ and find the terrain type you are leaving. Read across to the 'Lost' column entry. Roll two die. If the dice total equals or exceeds the chart's number, your party is lost. If you move more than one hex in a day, you must check for getting lost before each move, i.e., before you enter the new hex.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;If you get lost, you cannot move further that day. You are stuck in the hex you tried to leave. You must check for a travel event unless performing self-guiding moves
+ &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR205b' Content='r205b' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+ The travel check is performed in the hex you tried to enter, as if you actually entered it. This reflects you wondering around the edges of the new hex and perhaps encountering something.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR205a' Content='r205a' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Local Guide&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR205b1' Content='r205b' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Self-Guiding Moves&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR205c' Content='r205c' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Airborne&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR205d' Content='r205d' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; River Crossing</t>
   </si>
 </sst>
 </file>
@@ -3650,8 +3650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B229"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3662,426 +3662,426 @@
   <sheetData>
     <row r="1" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>348</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="240" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>356</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="157.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="360" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="375" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -4089,7 +4089,7 @@
         <v>19</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -4097,7 +4097,7 @@
         <v>17</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -4105,7 +4105,7 @@
         <v>18</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -4113,15 +4113,15 @@
         <v>0</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -4129,55 +4129,55 @@
         <v>16</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>203</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -4185,7 +4185,7 @@
         <v>21</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>197</v>
+        <v>457</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -4209,7 +4209,7 @@
         <v>24</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -4225,7 +4225,7 @@
         <v>26</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -4233,7 +4233,7 @@
         <v>27</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
@@ -4249,7 +4249,7 @@
         <v>29</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -4257,7 +4257,7 @@
         <v>30</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -4265,7 +4265,7 @@
         <v>31</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="330" x14ac:dyDescent="0.25">
@@ -4273,7 +4273,7 @@
         <v>32</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -4281,7 +4281,7 @@
         <v>33</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="360" x14ac:dyDescent="0.25">
@@ -4289,7 +4289,7 @@
         <v>34</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="360" x14ac:dyDescent="0.25">
@@ -4385,7 +4385,7 @@
         <v>46</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -4406,10 +4406,10 @@
     </row>
     <row r="94" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -4417,7 +4417,7 @@
         <v>51</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -4457,7 +4457,7 @@
         <v>8</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -4489,7 +4489,7 @@
         <v>12</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -4497,7 +4497,7 @@
         <v>13</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -4537,7 +4537,7 @@
         <v>3</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -4553,7 +4553,7 @@
         <v>53</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -4561,7 +4561,7 @@
         <v>69</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -4569,7 +4569,7 @@
         <v>70</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -4577,7 +4577,7 @@
         <v>71</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -4585,7 +4585,7 @@
         <v>72</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -4665,7 +4665,7 @@
         <v>84</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -4673,7 +4673,7 @@
         <v>85</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -4697,7 +4697,7 @@
         <v>89</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -4726,410 +4726,410 @@
     </row>
     <row r="134" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B134" s="1" t="s">
         <v>213</v>
-      </c>
-      <c r="B134" s="1" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -5137,7 +5137,7 @@
         <v>193</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -5353,7 +5353,7 @@
         <v>121</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="213" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -5377,7 +5377,7 @@
         <v>124</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -5457,7 +5457,7 @@
         <v>141</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="226" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -5465,7 +5465,7 @@
         <v>142</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="227" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -5473,7 +5473,7 @@
         <v>143</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="228" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -5481,7 +5481,7 @@
         <v>144</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -5489,7 +5489,7 @@
         <v>145</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix Resurrection Necklass Problem for Prince losing in combat. Add logging for GameFeats.
</commit_message>
<xml_diff>
--- a/DesignDocs/Rules.xlsx
+++ b/DesignDocs/Rules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\BarbarianPrince\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E1F7898-0D2F-43D6-B2B9-DFA524662143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D38BC94-CB60-4D7F-8052-75DD6122A7B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="1" r:id="rId1"/>
@@ -2100,19 +2100,6 @@
  &lt;InlineUIContainer&gt;&lt;Button Content='e065' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; - 6</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r202 The Barbarian Prince&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;You begin play as Cal Arath, rightful hier to the throne of the Northlands Kingdom. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt; - Few humans can match your skill with trusty Bonebitter, your broadsword -- you have a combat skill of eight. 
-&lt;LineBreak/&gt; - Life is the harsh northlands has developed your powerful body and magnificent physique -- you have endurance nine. 
-&lt;LineBreak/&gt; - Alas, in making your escape, you could only grab a few coins -- your wealth code is two. See
- &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR225' Content='r225' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
- to determine how many gold pieces you have taken.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-In addition, you have a 'wit and wiles' rating reflecting your ability to react quickly to situations, think your way out of trouble, and convince people to support your cause. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt; 
-Roll one die to determine this wit and wiles rating. If the result is one, consider it a two instead. If you have played the game before and won, you may wish an extra challenge by using a wits and wiles rating one less than the previous value; if you lost in the previous game, use a wit and wiles one higher than the previous value.</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;r206 Transport&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;When travelling; any food, gold, and possessions acquired by events must be carried. Many of these items have a weight in units of  'loads'. You can only carry a certain number of loads. Anything else must be left behind. Objects left behind can be placed in a cache
  &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR214' Content='r214' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
@@ -3282,6 +3269,19 @@
  &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR205b1' Content='r205b' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Self-Guiding Moves&lt;LineBreak/&gt;
  &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR205c' Content='r205c' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Airborne&lt;LineBreak/&gt;
  &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR205d' Content='r205d' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; River Crossing</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r202 The Barbarian Prince&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;You begin play as Cal Arath, rightful heir to the throne of the Northlands Kingdom. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt; - Few humans can match your skill with trusty Bonebitter, your broadsword -- you have a combat skill of eight. 
+&lt;LineBreak/&gt; - Life is the harsh northlands has developed your powerful body and magnificent physique -- you have endurance nine. 
+&lt;LineBreak/&gt; - Alas, in making your escape, you could only grab a few coins -- your wealth code is two. See
+ &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR225' Content='r225' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+ to determine how many gold pieces you have taken.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+In addition, you have a 'wit and wiles' rating reflecting your ability to react quickly to situations, think your way out of trouble, and convince people to support your cause. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt; 
+Roll one die to determine this wit and wiles rating. If the result is one, consider it a two instead. If you have played the game before and won, you may wish an extra challenge by using a wits and wiles rating one less than the previous value; if you lost in the previous game, use a wit and wiles one higher than the previous value.</t>
   </si>
 </sst>
 </file>
@@ -3650,8 +3650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B229"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3662,426 +3662,426 @@
   <sheetData>
     <row r="1" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>347</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="240" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>355</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="157.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="360" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="375" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -4089,7 +4089,7 @@
         <v>19</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -4097,7 +4097,7 @@
         <v>17</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -4105,7 +4105,7 @@
         <v>18</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>314</v>
+        <v>457</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -4113,15 +4113,15 @@
         <v>0</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -4129,7 +4129,7 @@
         <v>16</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -4161,7 +4161,7 @@
         <v>204</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -4185,7 +4185,7 @@
         <v>21</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -4209,7 +4209,7 @@
         <v>24</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -4225,7 +4225,7 @@
         <v>26</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -4233,7 +4233,7 @@
         <v>27</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
@@ -4249,7 +4249,7 @@
         <v>29</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -4257,7 +4257,7 @@
         <v>30</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -4265,7 +4265,7 @@
         <v>31</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="330" x14ac:dyDescent="0.25">
@@ -4273,7 +4273,7 @@
         <v>32</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -4281,7 +4281,7 @@
         <v>33</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="360" x14ac:dyDescent="0.25">
@@ -4289,7 +4289,7 @@
         <v>34</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="360" x14ac:dyDescent="0.25">
@@ -4385,7 +4385,7 @@
         <v>46</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -4406,10 +4406,10 @@
     </row>
     <row r="94" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -4417,7 +4417,7 @@
         <v>51</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -4457,7 +4457,7 @@
         <v>8</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -4489,7 +4489,7 @@
         <v>12</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -4497,7 +4497,7 @@
         <v>13</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -4537,7 +4537,7 @@
         <v>3</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -4553,7 +4553,7 @@
         <v>53</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -4561,7 +4561,7 @@
         <v>69</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -4585,7 +4585,7 @@
         <v>72</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -4665,7 +4665,7 @@
         <v>84</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -4673,7 +4673,7 @@
         <v>85</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -4697,7 +4697,7 @@
         <v>89</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -5137,7 +5137,7 @@
         <v>193</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -5353,7 +5353,7 @@
         <v>121</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="213" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -5377,7 +5377,7 @@
         <v>124</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -5457,7 +5457,7 @@
         <v>141</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="226" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -5473,7 +5473,7 @@
         <v>143</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="228" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -5481,7 +5481,7 @@
         <v>144</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="60" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix the Duplicate Horses issue when TransferMounts() called.
</commit_message>
<xml_diff>
--- a/DesignDocs/Rules.xlsx
+++ b/DesignDocs/Rules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\BarbarianPrince\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{92544BE7-CD6F-40CC-9547-0EBD5D3B3819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8CA45964-8F31-4A13-9E5A-AA4063D2C479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="16520" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="1" r:id="rId1"/>
@@ -377,10 +377,6 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;When the number of wounds to a character equals or exceeds half his endurance, he is seriously wounded. His combat strikes descreases two.</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r221c Death&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;When the number of wounds finally equals the endurance value fo the character, or exceeds it, the character dies. If the Barbarian Prince dies, the game is lost!</t>
-  </si>
-  <si>
     <t>r225</t>
   </si>
   <si>
@@ -706,14 +702,6 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;If anything else occurs, the battle continues. You can attempt to escape as often as your wish until you finally succeed.</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;Bold&gt;r220g Routes&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;If you wish, you can attempt to frighten your enemy into running away from the combat. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Roll one die each time you kill one character in the enemy group and after you finish all strikes.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;If a six occurs, the enemy routes and the battle ends.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;All surviving enemy characters flee and disapper so you cannot take their wealth. Otherwise, it is just as if you killed them all. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Opposing characters with a combat skill or endurance of 9+ are never subject to route. They will always fight to the death. </t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;r225b Distributing Acquisitions&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;You decide which characters receive his personal property. You can never take it back unless the character dies. At this point, you can recover his wealth unless you had to escape from the event or have already left.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;&lt;Italic&gt;Historical Note: This system for holding wealth is based on ancient Celtic and Germanic social customs. The chief or leader owned all the property including spoils from raids and wars. His band of followers were fed and housed. From time to time, they were given individual items as gifts for especially valuable services.&lt;/Italic&gt;</t>
@@ -2217,18 +2205,6 @@
   </si>
   <si>
     <t>r182</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r220 Combat&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;When your character and your party must fight characters encounted, these rules are used. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button Content='r220a' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Combat Procedure&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button Content='r220b' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Selecting Opponents&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button Content='r220c' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Strikes&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button Content='r220d' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Combat Table&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button Content='r220e' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Surprise&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button Content='r220f' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Escape&lt;LineBreak/&gt;
- &lt;InlineUIContainer&gt;&lt;Button Content='r220g' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Routs&lt;LineBreak/&gt;</t>
   </si>
   <si>
     <t>r180</t>
@@ -3293,6 +3269,30 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;If there is insufficient food for all, either you withhold it from all (including yourself) or share out what is available to all (this prevents the effects of character starvation
  &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR216b1' Content='r216b' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;).
  However, this does not eliminate the risk of desertion described above with character starvation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;r220g Routes&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;If you wish, you can attempt to frighten your enemy into running away from the combat. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Roll one die each time you kill one character in the enemy group and after you finish all strikes.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;If a six occurs, the enemy routes and the battle ends.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;All surviving enemy characters flee and disappear so you cannot take their wealth. Otherwise, it is just as if you killed them all. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Opposing characters with a combat skill or endurance of 9+ are never subject to route. They will always fight to the death. </t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r221c Death&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;When the number of wounds finally equals the endurance value of the character, or exceeds it, the character dies. If the Barbarian Prince dies, the game is lost!</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r220 Combat&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;When your character and your party must fight characters encounted, these rules are used. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button Content='r220a' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Combat Procedure&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button Content='r220b' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Selecting Opponents&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button Content='r220c' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Strikes&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button Content='r220d' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Combat Table&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button Content='r220e' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Surprise&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button Content='r220f' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Escape&lt;LineBreak/&gt;
+ &lt;InlineUIContainer&gt;&lt;Button Content='r220g' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Routs&lt;LineBreak/&gt;</t>
   </si>
 </sst>
 </file>
@@ -3661,553 +3661,553 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B102" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B104" sqref="B104"/>
+    <sheetView tabSelected="1" topLeftCell="B113" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B114" sqref="B114"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
-    <col min="2" max="2" width="231.5546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.125" style="2"/>
+    <col min="2" max="2" width="231.5" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="214" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>345</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="B6" s="1" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="157.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="B29" s="1" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="342.35" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="216" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="B31" s="1" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="356.6" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="214" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>396</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>370</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>382</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="144" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>353</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="157.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>356</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>371</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>362</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
-        <v>379</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
-        <v>365</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="345.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="360" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
-        <v>386</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
-        <v>456</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
-        <v>399</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="216" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A40" s="2" t="s">
-        <v>332</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
-        <v>335</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A45" s="2" t="s">
+      <c r="B51" s="1" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="214" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A49" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="B49" s="1" t="s">
+      <c r="B52" s="1" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A50" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="B50" s="1" t="s">
+    <row r="53" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A51" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="B51" s="1" t="s">
+    <row r="54" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="216" x14ac:dyDescent="0.3">
-      <c r="A52" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A53" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" ht="144" x14ac:dyDescent="0.3">
-      <c r="A54" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="360" x14ac:dyDescent="0.3">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="356.6" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="B61" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A62" s="2" t="s">
+      <c r="B63" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B62" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A63" s="2" t="s">
+    </row>
+    <row r="64" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B64" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="214" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A64" s="2" t="s">
+      <c r="B65" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" ht="216" x14ac:dyDescent="0.3">
-      <c r="A65" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="B65" s="1" t="s">
+      <c r="B66" s="1" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A66" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>22</v>
       </c>
@@ -4215,7 +4215,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>23</v>
       </c>
@@ -4223,15 +4223,15 @@
         <v>56</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>25</v>
       </c>
@@ -4239,23 +4239,23 @@
         <v>55</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>28</v>
       </c>
@@ -4263,63 +4263,63 @@
         <v>57</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="316.8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" ht="313.85000000000002" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="242.5" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" ht="316.8" x14ac:dyDescent="0.3">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="313.85000000000002" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" ht="345.6" x14ac:dyDescent="0.3">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="342.35" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" ht="345.6" x14ac:dyDescent="0.3">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="342.35" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="242.5" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>36</v>
       </c>
@@ -4327,15 +4327,15 @@
         <v>63</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>38</v>
       </c>
@@ -4343,7 +4343,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>39</v>
       </c>
@@ -4351,7 +4351,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>40</v>
       </c>
@@ -4359,7 +4359,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>41</v>
       </c>
@@ -4367,7 +4367,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>42</v>
       </c>
@@ -4375,7 +4375,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>43</v>
       </c>
@@ -4383,7 +4383,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>44</v>
       </c>
@@ -4391,71 +4391,71 @@
         <v>68</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" ht="288" x14ac:dyDescent="0.3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="285.3" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>6</v>
       </c>
@@ -4463,7 +4463,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>7</v>
       </c>
@@ -4471,23 +4471,23 @@
         <v>61</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>10</v>
       </c>
@@ -4495,7 +4495,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>11</v>
       </c>
@@ -4503,31 +4503,31 @@
         <v>20</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>15</v>
       </c>
@@ -4535,87 +4535,87 @@
         <v>62</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>74</v>
       </c>
@@ -4623,31 +4623,31 @@
         <v>77</v>
       </c>
     </row>
-    <row r="120" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>75</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>79</v>
       </c>
@@ -4655,860 +4655,860 @@
         <v>82</v>
       </c>
     </row>
-    <row r="124" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>81</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" ht="154.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" ht="154.55000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
+      <c r="A128" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B127" s="1" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A128" s="2" t="s">
+      <c r="B128" s="1" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
+      <c r="A129" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B128" s="1" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A129" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="B129" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
+      <c r="A130" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
+      <c r="A131" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
+      <c r="A132" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="A133" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
+      <c r="A134" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B134" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="130" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A130" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B130" s="1" t="s">
+    <row r="135" spans="1:2" ht="214" x14ac:dyDescent="0.25">
+      <c r="A135" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A136" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A137" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A138" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A139" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A140" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A141" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A142" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A143" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A144" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A145" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A146" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A147" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A148" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A149" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A150" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A151" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A152" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A153" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A154" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A155" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A156" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A157" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A158" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A159" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A160" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A161" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A162" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A163" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A164" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A165" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A166" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A167" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A168" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A169" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A170" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A171" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A172" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A173" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A174" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A175" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A176" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A177" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A178" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A179" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A180" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A181" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A182" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A183" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A184" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A185" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
+      <c r="A186" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
+      <c r="A187" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
+      <c r="A188" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
+      <c r="A189" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
+      <c r="A190" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
+      <c r="A191" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
+      <c r="A192" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
+      <c r="A193" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
+      <c r="A194" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
+      <c r="A195" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
+      <c r="A196" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B196" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="131" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A131" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B131" s="1" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" ht="144" x14ac:dyDescent="0.3">
-      <c r="A132" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B132" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A133" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B133" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A134" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B134" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" ht="216" x14ac:dyDescent="0.3">
-      <c r="A135" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="B135" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A136" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="B136" s="1" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A137" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="B137" s="1" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A138" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="B138" s="1" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A139" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="B139" s="1" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A140" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="B140" s="1" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A141" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="B141" s="1" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A142" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="B142" s="1" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A143" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="B143" s="1" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A144" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="B144" s="1" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A145" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="B145" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A146" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="B146" s="1" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A147" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="B147" s="1" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A148" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="B148" s="1" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A149" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="B149" s="1" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A150" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="B150" s="1" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A151" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="B151" s="1" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A152" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="B152" s="1" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A153" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="B153" s="1" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A154" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="B154" s="1" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A155" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="B155" s="1" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A156" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="B156" s="1" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A157" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="B157" s="1" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A158" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="B158" s="1" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A159" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="B159" s="1" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A160" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="B160" s="1" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A161" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="B161" s="1" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A162" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="B162" s="1" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A163" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="B163" s="1" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A164" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="B164" s="1" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A165" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="B165" s="1" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A166" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="B166" s="1" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A167" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="B167" s="1" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A168" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="B168" s="1" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A169" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="B169" s="1" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A170" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="B170" s="1" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A171" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="B171" s="1" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A172" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="B172" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A173" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="B173" s="1" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A174" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="B174" s="1" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A175" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="B175" s="1" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A176" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="B176" s="1" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A177" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="B177" s="1" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A178" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="B178" s="1" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A179" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="B179" s="1" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A180" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="B180" s="1" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A181" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="B181" s="1" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A182" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="B182" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="183" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A183" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="B183" s="1" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="184" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A184" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="B184" s="1" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="185" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A185" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="B185" s="1" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="186" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A186" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="B186" s="1" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="187" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A187" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B187" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="188" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A188" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B188" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="189" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A189" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B189" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="190" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A190" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B190" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="191" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A191" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B191" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="192" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A192" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B192" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="193" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A193" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B193" s="1" t="s">
+    <row r="197" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
+      <c r="A197" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B197" s="1" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="194" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A194" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B194" s="1" t="s">
+    <row r="198" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
+      <c r="A198" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
+      <c r="A199" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B199" s="1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="195" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A195" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B195" s="1" t="s">
+    <row r="200" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
+      <c r="A200" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
+      <c r="A201" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
+      <c r="A202" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
+      <c r="A203" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
+      <c r="A204" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
+      <c r="A205" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
+      <c r="A206" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B206" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
+      <c r="A207" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B207" s="1" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="196" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A196" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B196" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="197" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A197" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B197" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="198" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A198" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B198" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="199" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A199" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B199" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="200" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A200" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B200" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="201" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A201" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B201" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="202" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A202" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B202" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="203" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A203" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B203" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="204" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A204" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B204" s="1" t="s">
+    <row r="208" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
+      <c r="A208" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
+      <c r="A209" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
+      <c r="A210" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
+      <c r="A211" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B211" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="205" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A205" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B205" s="1" t="s">
+    <row r="212" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="A212" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
+      <c r="A213" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B213" s="1" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
+      <c r="A214" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B214" s="1" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="206" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A206" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B206" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="207" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A207" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B207" s="1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="208" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A208" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B208" s="1" t="s">
+    <row r="215" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
+      <c r="A215" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B215" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
+      <c r="A216" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B216" s="1" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" ht="214" x14ac:dyDescent="0.25">
+      <c r="A217" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B217" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
+      <c r="A218" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B218" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A219" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B219" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
+      <c r="A220" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B220" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
+      <c r="A221" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B221" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="A222" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B222" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
+      <c r="A223" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B223" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" ht="228.25" x14ac:dyDescent="0.25">
+      <c r="A224" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B224" s="1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="209" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A209" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B209" s="1" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="210" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A210" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B210" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="211" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A211" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B211" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="212" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A212" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B212" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="213" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A213" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="B213" s="1" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="214" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A214" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B214" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="215" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A215" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B215" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="216" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A216" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B216" s="1" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="217" spans="1:2" ht="216" x14ac:dyDescent="0.3">
-      <c r="A217" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="B217" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="218" spans="1:2" ht="144" x14ac:dyDescent="0.3">
-      <c r="A218" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B218" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="219" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A219" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B219" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="220" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A220" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B220" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="221" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A221" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B221" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="222" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A222" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B222" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="223" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A223" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B223" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="224" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
-      <c r="A224" s="2" t="s">
+    <row r="225" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
+      <c r="A225" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B224" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="225" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A225" s="2" t="s">
+      <c r="B225" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B225" s="1" t="s">
+    </row>
+    <row r="226" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
+      <c r="A226" s="2" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="226" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A226" s="2" t="s">
+      <c r="B226" s="1" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" ht="128.4" x14ac:dyDescent="0.25">
+      <c r="A227" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B226" s="1" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="227" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A227" s="2" t="s">
+      <c r="B227" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" ht="370.9" x14ac:dyDescent="0.25">
+      <c r="A228" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="B227" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="228" spans="1:2" ht="374.4" x14ac:dyDescent="0.3">
-      <c r="A228" s="2" t="s">
+      <c r="B228" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" ht="370.9" x14ac:dyDescent="0.25">
+      <c r="A229" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B228" s="1" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="229" spans="1:2" ht="374.4" x14ac:dyDescent="0.3">
-      <c r="A229" s="2" t="s">
+      <c r="B229" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
+      <c r="A230" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B229" s="1" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="230" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A230" s="2" t="s">
-        <v>145</v>
-      </c>
       <c r="B230" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>